<commit_message>
Fix category sales GMV formatting and add GMV KPI in AMS trend
</commit_message>
<xml_diff>
--- a/data/raw/sales/Week 6/Audio_Array/other_channels.xlsx
+++ b/data/raw/sales/Week 6/Audio_Array/other_channels.xlsx
@@ -5,12 +5,12 @@
   <workbookPr hidePivotFieldList="1" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Admin\OneDrive\Desktop\New folder\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\Other computers\My Laptop\D\Nitesh\Weekly Report - B2B + B2C\FastAPI\data\raw\sales\Week 6\Audio_Array\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{10431519-7B97-4569-8C70-21DF7D663AC1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{50DBBB52-1185-44FC-AB17-0ED38EDB3766}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="3" xr2:uid="{00DB3424-A17B-4A18-BC6A-329A1F1119CF}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="4" xr2:uid="{00DB3424-A17B-4A18-BC6A-329A1F1119CF}"/>
   </bookViews>
   <sheets>
     <sheet name="D2C - Audio Array" sheetId="4" r:id="rId1"/>
@@ -21,7 +21,7 @@
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="3" hidden="1">'1p Sales'!$A$1:$G$1</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="4" hidden="1">B2B!$A$1:$F$33</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="4" hidden="1">B2B!$A$1:$F$32</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">'BI Worldwide'!$A$1:$E$5</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">'Blinkit Sales'!$A$1:$F$5</definedName>
   </definedNames>
@@ -44,7 +44,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="697" uniqueCount="364">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="693" uniqueCount="362">
   <si>
     <t>Brand</t>
   </si>
@@ -605,12 +605,6 @@
   </si>
   <si>
     <t>Enertia</t>
-  </si>
-  <si>
-    <t>FBA79590</t>
-  </si>
-  <si>
-    <t>CFM-01</t>
   </si>
   <si>
     <t>FBA79005</t>
@@ -1663,10 +1657,10 @@
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A3" s="19" t="s">
-        <v>241</v>
+        <v>239</v>
       </c>
       <c r="B3" s="19" t="s">
-        <v>242</v>
+        <v>240</v>
       </c>
       <c r="C3" s="19">
         <v>3</v>
@@ -1680,10 +1674,10 @@
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A4" s="19" t="s">
-        <v>243</v>
+        <v>241</v>
       </c>
       <c r="B4" s="19" t="s">
-        <v>244</v>
+        <v>242</v>
       </c>
       <c r="C4" s="19">
         <v>1</v>
@@ -1697,10 +1691,10 @@
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A5" s="19" t="s">
-        <v>245</v>
+        <v>243</v>
       </c>
       <c r="B5" s="19" t="s">
-        <v>246</v>
+        <v>244</v>
       </c>
       <c r="C5" s="19">
         <v>1</v>
@@ -1714,10 +1708,10 @@
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A6" s="19" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
       <c r="B6" s="19" t="s">
-        <v>248</v>
+        <v>246</v>
       </c>
       <c r="C6" s="19">
         <v>2</v>
@@ -1731,10 +1725,10 @@
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A7" s="19" t="s">
-        <v>249</v>
+        <v>247</v>
       </c>
       <c r="B7" s="19" t="s">
-        <v>250</v>
+        <v>248</v>
       </c>
       <c r="C7" s="19">
         <v>1</v>
@@ -1748,10 +1742,10 @@
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A8" s="19" t="s">
-        <v>199</v>
+        <v>197</v>
       </c>
       <c r="B8" s="19" t="s">
-        <v>200</v>
+        <v>198</v>
       </c>
       <c r="C8" s="19">
         <v>1</v>
@@ -1765,10 +1759,10 @@
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A9" s="19" t="s">
-        <v>251</v>
+        <v>249</v>
       </c>
       <c r="B9" s="19" t="s">
-        <v>252</v>
+        <v>250</v>
       </c>
       <c r="C9" s="19">
         <v>1</v>
@@ -1782,10 +1776,10 @@
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A10" s="19" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
       <c r="B10" s="19" t="s">
-        <v>253</v>
+        <v>251</v>
       </c>
       <c r="C10" s="19">
         <v>22</v>
@@ -1799,10 +1793,10 @@
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A11" s="19" t="s">
-        <v>254</v>
+        <v>252</v>
       </c>
       <c r="B11" s="19" t="s">
-        <v>255</v>
+        <v>253</v>
       </c>
       <c r="C11" s="19">
         <v>1</v>
@@ -1816,10 +1810,10 @@
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A12" s="19" t="s">
-        <v>201</v>
+        <v>199</v>
       </c>
       <c r="B12" s="19" t="s">
-        <v>202</v>
+        <v>200</v>
       </c>
       <c r="C12" s="19">
         <v>2</v>
@@ -1833,10 +1827,10 @@
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A13" s="19" t="s">
-        <v>256</v>
+        <v>254</v>
       </c>
       <c r="B13" s="19" t="s">
-        <v>257</v>
+        <v>255</v>
       </c>
       <c r="C13" s="19">
         <v>3</v>
@@ -1850,10 +1844,10 @@
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A14" s="19" t="s">
-        <v>203</v>
+        <v>201</v>
       </c>
       <c r="B14" s="19" t="s">
-        <v>204</v>
+        <v>202</v>
       </c>
       <c r="C14" s="19">
         <v>6</v>
@@ -1867,10 +1861,10 @@
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A15" s="19" t="s">
-        <v>258</v>
+        <v>256</v>
       </c>
       <c r="B15" s="19" t="s">
-        <v>244</v>
+        <v>242</v>
       </c>
       <c r="C15" s="19">
         <v>5</v>
@@ -1884,10 +1878,10 @@
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A16" s="19" t="s">
-        <v>259</v>
+        <v>257</v>
       </c>
       <c r="B16" s="19" t="s">
-        <v>260</v>
+        <v>258</v>
       </c>
       <c r="C16" s="19">
         <v>5</v>
@@ -1901,10 +1895,10 @@
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A17" s="19" t="s">
-        <v>261</v>
+        <v>259</v>
       </c>
       <c r="B17" s="19" t="s">
-        <v>262</v>
+        <v>260</v>
       </c>
       <c r="C17" s="19">
         <v>3</v>
@@ -1918,10 +1912,10 @@
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A18" s="19" t="s">
-        <v>207</v>
+        <v>205</v>
       </c>
       <c r="B18" s="19" t="s">
-        <v>208</v>
+        <v>206</v>
       </c>
       <c r="C18" s="19">
         <v>3</v>
@@ -1935,10 +1929,10 @@
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A19" s="19" t="s">
-        <v>263</v>
+        <v>261</v>
       </c>
       <c r="B19" s="19" t="s">
-        <v>264</v>
+        <v>262</v>
       </c>
       <c r="C19" s="19">
         <v>3</v>
@@ -1952,10 +1946,10 @@
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A20" s="19" t="s">
-        <v>265</v>
+        <v>263</v>
       </c>
       <c r="B20" s="19" t="s">
-        <v>266</v>
+        <v>264</v>
       </c>
       <c r="C20" s="19">
         <v>3</v>
@@ -1969,10 +1963,10 @@
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A21" s="19" t="s">
-        <v>209</v>
+        <v>207</v>
       </c>
       <c r="B21" s="19" t="s">
-        <v>210</v>
+        <v>208</v>
       </c>
       <c r="C21" s="19">
         <v>4</v>
@@ -1986,10 +1980,10 @@
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A22" s="19" t="s">
-        <v>211</v>
+        <v>209</v>
       </c>
       <c r="B22" s="19" t="s">
-        <v>212</v>
+        <v>210</v>
       </c>
       <c r="C22" s="19">
         <v>6</v>
@@ -2020,10 +2014,10 @@
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A24" s="19" t="s">
-        <v>267</v>
+        <v>265</v>
       </c>
       <c r="B24" s="19" t="s">
-        <v>268</v>
+        <v>266</v>
       </c>
       <c r="C24" s="19">
         <v>3</v>
@@ -2037,10 +2031,10 @@
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A25" s="19" t="s">
-        <v>269</v>
+        <v>267</v>
       </c>
       <c r="B25" s="19" t="s">
-        <v>270</v>
+        <v>268</v>
       </c>
       <c r="C25" s="19">
         <v>5</v>
@@ -2071,7 +2065,7 @@
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A27" s="19" t="s">
-        <v>215</v>
+        <v>213</v>
       </c>
       <c r="B27" s="19" t="s">
         <v>185</v>
@@ -2088,10 +2082,10 @@
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A28" s="19" t="s">
-        <v>216</v>
+        <v>214</v>
       </c>
       <c r="B28" s="19" t="s">
-        <v>217</v>
+        <v>215</v>
       </c>
       <c r="C28" s="19">
         <v>26</v>
@@ -2105,10 +2099,10 @@
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A29" s="19" t="s">
-        <v>237</v>
+        <v>235</v>
       </c>
       <c r="B29" s="19" t="s">
-        <v>238</v>
+        <v>236</v>
       </c>
       <c r="C29" s="19">
         <v>5</v>
@@ -2122,10 +2116,10 @@
     </row>
     <row r="30" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A30" s="19" t="s">
-        <v>239</v>
+        <v>237</v>
       </c>
       <c r="B30" s="19" t="s">
-        <v>240</v>
+        <v>238</v>
       </c>
       <c r="C30" s="19">
         <v>16</v>
@@ -2139,10 +2133,10 @@
     </row>
     <row r="31" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A31" s="19" t="s">
-        <v>271</v>
+        <v>269</v>
       </c>
       <c r="B31" s="19" t="s">
-        <v>272</v>
+        <v>270</v>
       </c>
       <c r="C31" s="19">
         <v>2</v>
@@ -2156,10 +2150,10 @@
     </row>
     <row r="32" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A32" s="19" t="s">
-        <v>218</v>
+        <v>216</v>
       </c>
       <c r="B32" s="19" t="s">
-        <v>273</v>
+        <v>271</v>
       </c>
       <c r="C32" s="19">
         <v>7</v>
@@ -2173,10 +2167,10 @@
     </row>
     <row r="33" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A33" s="19" t="s">
-        <v>232</v>
+        <v>230</v>
       </c>
       <c r="B33" s="19" t="s">
-        <v>260</v>
+        <v>258</v>
       </c>
       <c r="C33" s="19">
         <v>1</v>
@@ -2190,10 +2184,10 @@
     </row>
     <row r="34" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A34" s="19" t="s">
-        <v>220</v>
+        <v>218</v>
       </c>
       <c r="B34" s="19" t="s">
-        <v>221</v>
+        <v>219</v>
       </c>
       <c r="C34" s="19">
         <v>3</v>
@@ -2207,10 +2201,10 @@
     </row>
     <row r="35" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A35" s="19" t="s">
-        <v>274</v>
+        <v>272</v>
       </c>
       <c r="B35" s="19" t="s">
-        <v>275</v>
+        <v>273</v>
       </c>
       <c r="C35" s="19">
         <v>30</v>
@@ -2285,10 +2279,10 @@
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A3" s="2" t="s">
-        <v>235</v>
+        <v>233</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>236</v>
+        <v>234</v>
       </c>
       <c r="C3" s="2">
         <v>2</v>
@@ -2302,10 +2296,10 @@
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A4" s="2" t="s">
-        <v>237</v>
+        <v>235</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>238</v>
+        <v>236</v>
       </c>
       <c r="C4" s="2">
         <v>1</v>
@@ -2319,10 +2313,10 @@
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A5" s="2" t="s">
-        <v>239</v>
+        <v>237</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>240</v>
+        <v>238</v>
       </c>
       <c r="C5" s="2">
         <v>2</v>
@@ -2419,13 +2413,13 @@
         <v>11</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>207</v>
+        <v>205</v>
       </c>
       <c r="C2" s="2" t="s">
         <v>134</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>208</v>
+        <v>206</v>
       </c>
       <c r="E2" s="13">
         <v>17</v>
@@ -2459,13 +2453,13 @@
         <v>11</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>276</v>
+        <v>274</v>
       </c>
       <c r="C4" s="2" t="s">
         <v>16</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>277</v>
+        <v>275</v>
       </c>
       <c r="E4" s="13">
         <v>2</v>
@@ -2479,13 +2473,13 @@
         <v>11</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>263</v>
+        <v>261</v>
       </c>
       <c r="C5" s="2" t="s">
         <v>138</v>
       </c>
       <c r="D5" s="2" t="s">
-        <v>264</v>
+        <v>262</v>
       </c>
       <c r="E5" s="13">
         <v>1</v>
@@ -2503,7 +2497,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AEFCE879-280C-4E5F-92D0-2856EC6FD320}">
   <dimension ref="A1:G83"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="G1" sqref="G1"/>
     </sheetView>
   </sheetViews>
@@ -2541,10 +2535,10 @@
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
       <c r="B2" t="s">
-        <v>192</v>
+        <v>190</v>
       </c>
       <c r="C2" s="15" t="s">
         <v>9</v>
@@ -2587,10 +2581,10 @@
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>267</v>
+        <v>265</v>
       </c>
       <c r="B4" t="s">
-        <v>268</v>
+        <v>266</v>
       </c>
       <c r="C4" s="15" t="s">
         <v>14</v>
@@ -2610,10 +2604,10 @@
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>276</v>
+        <v>274</v>
       </c>
       <c r="B5" t="s">
-        <v>277</v>
+        <v>275</v>
       </c>
       <c r="C5" s="15" t="s">
         <v>16</v>
@@ -2656,10 +2650,10 @@
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>278</v>
+        <v>276</v>
       </c>
       <c r="B7" t="s">
-        <v>279</v>
+        <v>277</v>
       </c>
       <c r="C7" s="15" t="s">
         <v>20</v>
@@ -2679,10 +2673,10 @@
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>280</v>
+        <v>278</v>
       </c>
       <c r="B8" t="s">
-        <v>281</v>
+        <v>279</v>
       </c>
       <c r="C8" s="15" t="s">
         <v>22</v>
@@ -2702,10 +2696,10 @@
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
-        <v>203</v>
+        <v>201</v>
       </c>
       <c r="B9" t="s">
-        <v>204</v>
+        <v>202</v>
       </c>
       <c r="C9" s="15" t="s">
         <v>24</v>
@@ -2725,10 +2719,10 @@
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
-        <v>282</v>
+        <v>280</v>
       </c>
       <c r="B10" t="s">
-        <v>283</v>
+        <v>281</v>
       </c>
       <c r="C10" s="15" t="s">
         <v>26</v>
@@ -2748,10 +2742,10 @@
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
-        <v>284</v>
+        <v>282</v>
       </c>
       <c r="B11" t="s">
-        <v>285</v>
+        <v>283</v>
       </c>
       <c r="C11" s="15" t="s">
         <v>28</v>
@@ -2771,10 +2765,10 @@
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
-        <v>241</v>
+        <v>239</v>
       </c>
       <c r="B12" t="s">
-        <v>286</v>
+        <v>284</v>
       </c>
       <c r="C12" s="15" t="s">
         <v>30</v>
@@ -2794,10 +2788,10 @@
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
       <c r="B13" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
       <c r="C13" s="15" t="s">
         <v>32</v>
@@ -2817,10 +2811,10 @@
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
-        <v>287</v>
+        <v>285</v>
       </c>
       <c r="B14" t="s">
-        <v>288</v>
+        <v>286</v>
       </c>
       <c r="C14" s="15" t="s">
         <v>34</v>
@@ -2840,10 +2834,10 @@
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
-        <v>289</v>
+        <v>287</v>
       </c>
       <c r="B15" t="s">
-        <v>290</v>
+        <v>288</v>
       </c>
       <c r="C15" s="15" t="s">
         <v>36</v>
@@ -2863,10 +2857,10 @@
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
-        <v>251</v>
+        <v>249</v>
       </c>
       <c r="B16" t="s">
-        <v>252</v>
+        <v>250</v>
       </c>
       <c r="C16" s="15" t="s">
         <v>38</v>
@@ -2886,10 +2880,10 @@
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
-        <v>291</v>
+        <v>289</v>
       </c>
       <c r="B17" t="s">
-        <v>292</v>
+        <v>290</v>
       </c>
       <c r="C17" s="15" t="s">
         <v>40</v>
@@ -2909,10 +2903,10 @@
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
-        <v>293</v>
+        <v>291</v>
       </c>
       <c r="B18" t="s">
-        <v>294</v>
+        <v>292</v>
       </c>
       <c r="C18" s="15" t="s">
         <v>42</v>
@@ -2932,10 +2926,10 @@
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
-        <v>295</v>
+        <v>293</v>
       </c>
       <c r="B19" t="s">
-        <v>296</v>
+        <v>294</v>
       </c>
       <c r="C19" s="15" t="s">
         <v>44</v>
@@ -2955,10 +2949,10 @@
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
-        <v>239</v>
+        <v>237</v>
       </c>
       <c r="B20" t="s">
-        <v>297</v>
+        <v>295</v>
       </c>
       <c r="C20" s="15" t="s">
         <v>46</v>
@@ -2978,10 +2972,10 @@
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
-        <v>298</v>
+        <v>296</v>
       </c>
       <c r="B21" t="s">
-        <v>299</v>
+        <v>297</v>
       </c>
       <c r="C21" s="15" t="s">
         <v>48</v>
@@ -3001,10 +2995,10 @@
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
-        <v>300</v>
+        <v>298</v>
       </c>
       <c r="B22" t="s">
-        <v>301</v>
+        <v>299</v>
       </c>
       <c r="C22" s="15" t="s">
         <v>50</v>
@@ -3024,10 +3018,10 @@
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
-        <v>269</v>
+        <v>267</v>
       </c>
       <c r="B23" t="s">
-        <v>270</v>
+        <v>268</v>
       </c>
       <c r="C23" s="15" t="s">
         <v>52</v>
@@ -3047,10 +3041,10 @@
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
-        <v>237</v>
+        <v>235</v>
       </c>
       <c r="B24" t="s">
-        <v>302</v>
+        <v>300</v>
       </c>
       <c r="C24" s="15" t="s">
         <v>54</v>
@@ -3070,10 +3064,10 @@
     </row>
     <row r="25" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
       <c r="B25" t="s">
-        <v>196</v>
+        <v>194</v>
       </c>
       <c r="C25" s="15" t="s">
         <v>56</v>
@@ -3093,10 +3087,10 @@
     </row>
     <row r="26" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
-        <v>216</v>
+        <v>214</v>
       </c>
       <c r="B26" t="s">
-        <v>217</v>
+        <v>215</v>
       </c>
       <c r="C26" s="15" t="s">
         <v>58</v>
@@ -3116,10 +3110,10 @@
     </row>
     <row r="27" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
-        <v>249</v>
+        <v>247</v>
       </c>
       <c r="B27" t="s">
-        <v>250</v>
+        <v>248</v>
       </c>
       <c r="C27" s="15" t="s">
         <v>60</v>
@@ -3139,10 +3133,10 @@
     </row>
     <row r="28" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
-        <v>197</v>
+        <v>195</v>
       </c>
       <c r="B28" t="s">
-        <v>198</v>
+        <v>196</v>
       </c>
       <c r="C28" s="15" t="s">
         <v>62</v>
@@ -3162,10 +3156,10 @@
     </row>
     <row r="29" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
-        <v>303</v>
+        <v>301</v>
       </c>
       <c r="B29" t="s">
-        <v>304</v>
+        <v>302</v>
       </c>
       <c r="C29" s="15" t="s">
         <v>64</v>
@@ -3185,10 +3179,10 @@
     </row>
     <row r="30" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
-        <v>261</v>
+        <v>259</v>
       </c>
       <c r="B30" t="s">
-        <v>262</v>
+        <v>260</v>
       </c>
       <c r="C30" s="15" t="s">
         <v>66</v>
@@ -3208,10 +3202,10 @@
     </row>
     <row r="31" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
-        <v>201</v>
+        <v>199</v>
       </c>
       <c r="B31" t="s">
-        <v>202</v>
+        <v>200</v>
       </c>
       <c r="C31" s="15" t="s">
         <v>68</v>
@@ -3231,10 +3225,10 @@
     </row>
     <row r="32" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
-        <v>305</v>
+        <v>303</v>
       </c>
       <c r="B32" t="s">
-        <v>306</v>
+        <v>304</v>
       </c>
       <c r="C32" s="15" t="s">
         <v>70</v>
@@ -3254,10 +3248,10 @@
     </row>
     <row r="33" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A33" t="s">
-        <v>245</v>
+        <v>243</v>
       </c>
       <c r="B33" t="s">
-        <v>246</v>
+        <v>244</v>
       </c>
       <c r="C33" s="15" t="s">
         <v>72</v>
@@ -3277,10 +3271,10 @@
     </row>
     <row r="34" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A34" t="s">
-        <v>307</v>
+        <v>305</v>
       </c>
       <c r="B34" t="s">
-        <v>308</v>
+        <v>306</v>
       </c>
       <c r="C34" s="15" t="s">
         <v>74</v>
@@ -3300,10 +3294,10 @@
     </row>
     <row r="35" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A35" t="s">
-        <v>205</v>
+        <v>203</v>
       </c>
       <c r="B35" t="s">
-        <v>206</v>
+        <v>204</v>
       </c>
       <c r="C35" s="15" t="s">
         <v>76</v>
@@ -3323,10 +3317,10 @@
     </row>
     <row r="36" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A36" t="s">
-        <v>309</v>
+        <v>307</v>
       </c>
       <c r="B36" t="s">
-        <v>310</v>
+        <v>308</v>
       </c>
       <c r="C36" s="15" t="s">
         <v>78</v>
@@ -3346,10 +3340,10 @@
     </row>
     <row r="37" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A37" t="s">
-        <v>209</v>
+        <v>207</v>
       </c>
       <c r="B37" t="s">
-        <v>210</v>
+        <v>208</v>
       </c>
       <c r="C37" s="15" t="s">
         <v>80</v>
@@ -3369,10 +3363,10 @@
     </row>
     <row r="38" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A38" t="s">
-        <v>311</v>
+        <v>309</v>
       </c>
       <c r="B38" t="s">
-        <v>312</v>
+        <v>310</v>
       </c>
       <c r="C38" s="15" t="s">
         <v>82</v>
@@ -3392,10 +3386,10 @@
     </row>
     <row r="39" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A39" t="s">
-        <v>313</v>
+        <v>311</v>
       </c>
       <c r="B39" t="s">
-        <v>314</v>
+        <v>312</v>
       </c>
       <c r="C39" s="15" t="s">
         <v>84</v>
@@ -3415,10 +3409,10 @@
     </row>
     <row r="40" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A40" t="s">
-        <v>315</v>
+        <v>313</v>
       </c>
       <c r="B40" t="s">
-        <v>316</v>
+        <v>314</v>
       </c>
       <c r="C40" s="15" t="s">
         <v>86</v>
@@ -3438,10 +3432,10 @@
     </row>
     <row r="41" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A41" t="s">
-        <v>211</v>
+        <v>209</v>
       </c>
       <c r="B41" t="s">
-        <v>212</v>
+        <v>210</v>
       </c>
       <c r="C41" s="15" t="s">
         <v>88</v>
@@ -3461,10 +3455,10 @@
     </row>
     <row r="42" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A42" t="s">
-        <v>271</v>
+        <v>269</v>
       </c>
       <c r="B42" t="s">
-        <v>317</v>
+        <v>315</v>
       </c>
       <c r="C42" s="15" t="s">
         <v>90</v>
@@ -3484,10 +3478,10 @@
     </row>
     <row r="43" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A43" t="s">
-        <v>318</v>
+        <v>316</v>
       </c>
       <c r="B43" t="s">
-        <v>319</v>
+        <v>317</v>
       </c>
       <c r="C43" s="15" t="s">
         <v>92</v>
@@ -3507,10 +3501,10 @@
     </row>
     <row r="44" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A44" t="s">
-        <v>243</v>
+        <v>241</v>
       </c>
       <c r="B44" t="s">
-        <v>244</v>
+        <v>242</v>
       </c>
       <c r="C44" s="15" t="s">
         <v>94</v>
@@ -3530,10 +3524,10 @@
     </row>
     <row r="45" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A45" t="s">
-        <v>320</v>
+        <v>318</v>
       </c>
       <c r="B45" t="s">
-        <v>321</v>
+        <v>319</v>
       </c>
       <c r="C45" s="15" t="s">
         <v>96</v>
@@ -3553,10 +3547,10 @@
     </row>
     <row r="46" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A46" t="s">
-        <v>218</v>
+        <v>216</v>
       </c>
       <c r="B46" t="s">
-        <v>322</v>
+        <v>320</v>
       </c>
       <c r="C46" s="15" t="s">
         <v>98</v>
@@ -3576,10 +3570,10 @@
     </row>
     <row r="47" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A47" t="s">
-        <v>199</v>
+        <v>197</v>
       </c>
       <c r="B47" t="s">
-        <v>200</v>
+        <v>198</v>
       </c>
       <c r="C47" s="15" t="s">
         <v>100</v>
@@ -3599,10 +3593,10 @@
     </row>
     <row r="48" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A48" t="s">
-        <v>323</v>
+        <v>321</v>
       </c>
       <c r="B48" t="s">
-        <v>324</v>
+        <v>322</v>
       </c>
       <c r="C48" s="15" t="s">
         <v>102</v>
@@ -3622,10 +3616,10 @@
     </row>
     <row r="49" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A49" t="s">
-        <v>258</v>
+        <v>256</v>
       </c>
       <c r="B49" t="s">
-        <v>325</v>
+        <v>323</v>
       </c>
       <c r="C49" s="15" t="s">
         <v>104</v>
@@ -3645,10 +3639,10 @@
     </row>
     <row r="50" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A50" t="s">
-        <v>256</v>
+        <v>254</v>
       </c>
       <c r="B50" t="s">
-        <v>257</v>
+        <v>255</v>
       </c>
       <c r="C50" s="15" t="s">
         <v>106</v>
@@ -3668,10 +3662,10 @@
     </row>
     <row r="51" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A51" t="s">
-        <v>326</v>
+        <v>324</v>
       </c>
       <c r="B51" t="s">
-        <v>327</v>
+        <v>325</v>
       </c>
       <c r="C51" s="15" t="s">
         <v>108</v>
@@ -3691,10 +3685,10 @@
     </row>
     <row r="52" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A52" t="s">
-        <v>328</v>
+        <v>326</v>
       </c>
       <c r="B52" t="s">
-        <v>329</v>
+        <v>327</v>
       </c>
       <c r="C52" s="15" t="s">
         <v>110</v>
@@ -3714,7 +3708,7 @@
     </row>
     <row r="53" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A53" t="s">
-        <v>215</v>
+        <v>213</v>
       </c>
       <c r="B53" t="s">
         <v>185</v>
@@ -3737,10 +3731,10 @@
     </row>
     <row r="54" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A54" t="s">
-        <v>259</v>
+        <v>257</v>
       </c>
       <c r="B54" t="s">
-        <v>260</v>
+        <v>258</v>
       </c>
       <c r="C54" s="15" t="s">
         <v>114</v>
@@ -3760,10 +3754,10 @@
     </row>
     <row r="55" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A55" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
       <c r="B55" t="s">
-        <v>248</v>
+        <v>246</v>
       </c>
       <c r="C55" s="15" t="s">
         <v>116</v>
@@ -3783,10 +3777,10 @@
     </row>
     <row r="56" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A56" t="s">
-        <v>222</v>
+        <v>220</v>
       </c>
       <c r="B56" t="s">
-        <v>223</v>
+        <v>221</v>
       </c>
       <c r="C56" s="15" t="s">
         <v>118</v>
@@ -3806,10 +3800,10 @@
     </row>
     <row r="57" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A57" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
       <c r="B57" t="s">
-        <v>194</v>
+        <v>192</v>
       </c>
       <c r="C57" s="15" t="s">
         <v>120</v>
@@ -3829,10 +3823,10 @@
     </row>
     <row r="58" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A58" t="s">
-        <v>330</v>
+        <v>328</v>
       </c>
       <c r="B58" t="s">
-        <v>331</v>
+        <v>329</v>
       </c>
       <c r="C58" s="15" t="s">
         <v>122</v>
@@ -3852,10 +3846,10 @@
     </row>
     <row r="59" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A59" t="s">
-        <v>332</v>
+        <v>330</v>
       </c>
       <c r="B59" t="s">
-        <v>333</v>
+        <v>331</v>
       </c>
       <c r="C59" s="15" t="s">
         <v>124</v>
@@ -3875,10 +3869,10 @@
     </row>
     <row r="60" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A60" t="s">
-        <v>254</v>
+        <v>252</v>
       </c>
       <c r="B60" t="s">
-        <v>255</v>
+        <v>253</v>
       </c>
       <c r="C60" s="15" t="s">
         <v>126</v>
@@ -3898,10 +3892,10 @@
     </row>
     <row r="61" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A61" t="s">
-        <v>334</v>
+        <v>332</v>
       </c>
       <c r="B61" t="s">
-        <v>335</v>
+        <v>333</v>
       </c>
       <c r="C61" s="15" t="s">
         <v>128</v>
@@ -3921,10 +3915,10 @@
     </row>
     <row r="62" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A62" t="s">
-        <v>265</v>
+        <v>263</v>
       </c>
       <c r="B62" t="s">
-        <v>336</v>
+        <v>334</v>
       </c>
       <c r="C62" s="15" t="s">
         <v>130</v>
@@ -3944,10 +3938,10 @@
     </row>
     <row r="63" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A63" t="s">
-        <v>230</v>
+        <v>228</v>
       </c>
       <c r="B63" t="s">
-        <v>231</v>
+        <v>229</v>
       </c>
       <c r="C63" s="15" t="s">
         <v>132</v>
@@ -3967,10 +3961,10 @@
     </row>
     <row r="64" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A64" t="s">
-        <v>207</v>
+        <v>205</v>
       </c>
       <c r="B64" t="s">
-        <v>208</v>
+        <v>206</v>
       </c>
       <c r="C64" s="15" t="s">
         <v>134</v>
@@ -3993,7 +3987,7 @@
         <v>180</v>
       </c>
       <c r="B65" t="s">
-        <v>337</v>
+        <v>335</v>
       </c>
       <c r="C65" s="15" t="s">
         <v>136</v>
@@ -4013,10 +4007,10 @@
     </row>
     <row r="66" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A66" t="s">
-        <v>263</v>
+        <v>261</v>
       </c>
       <c r="B66" t="s">
-        <v>264</v>
+        <v>262</v>
       </c>
       <c r="C66" s="15" t="s">
         <v>138</v>
@@ -4036,10 +4030,10 @@
     </row>
     <row r="67" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A67" t="s">
-        <v>235</v>
+        <v>233</v>
       </c>
       <c r="B67" t="s">
-        <v>236</v>
+        <v>234</v>
       </c>
       <c r="C67" s="15" t="s">
         <v>140</v>
@@ -4059,10 +4053,10 @@
     </row>
     <row r="68" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A68" t="s">
-        <v>338</v>
+        <v>336</v>
       </c>
       <c r="B68" t="s">
-        <v>339</v>
+        <v>337</v>
       </c>
       <c r="C68" s="15" t="s">
         <v>142</v>
@@ -4082,10 +4076,10 @@
     </row>
     <row r="69" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A69" t="s">
-        <v>340</v>
+        <v>338</v>
       </c>
       <c r="B69" t="s">
-        <v>341</v>
+        <v>339</v>
       </c>
       <c r="C69" s="15" t="s">
         <v>144</v>
@@ -4105,10 +4099,10 @@
     </row>
     <row r="70" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A70" t="s">
-        <v>342</v>
+        <v>340</v>
       </c>
       <c r="B70" t="s">
-        <v>343</v>
+        <v>341</v>
       </c>
       <c r="C70" s="15" t="s">
         <v>146</v>
@@ -4128,10 +4122,10 @@
     </row>
     <row r="71" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A71" t="s">
-        <v>344</v>
+        <v>342</v>
       </c>
       <c r="B71" t="s">
-        <v>345</v>
+        <v>343</v>
       </c>
       <c r="C71" s="15" t="s">
         <v>148</v>
@@ -4151,10 +4145,10 @@
     </row>
     <row r="72" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A72" t="s">
-        <v>226</v>
+        <v>224</v>
       </c>
       <c r="B72" t="s">
-        <v>227</v>
+        <v>225</v>
       </c>
       <c r="C72" s="15" t="s">
         <v>150</v>
@@ -4174,10 +4168,10 @@
     </row>
     <row r="73" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A73" t="s">
-        <v>346</v>
+        <v>344</v>
       </c>
       <c r="B73" t="s">
-        <v>347</v>
+        <v>345</v>
       </c>
       <c r="C73" s="15" t="s">
         <v>152</v>
@@ -4197,10 +4191,10 @@
     </row>
     <row r="74" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A74" t="s">
-        <v>348</v>
+        <v>346</v>
       </c>
       <c r="B74" t="s">
-        <v>349</v>
+        <v>347</v>
       </c>
       <c r="C74" s="15" t="s">
         <v>154</v>
@@ -4220,10 +4214,10 @@
     </row>
     <row r="75" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A75" t="s">
-        <v>350</v>
+        <v>348</v>
       </c>
       <c r="B75" t="s">
-        <v>351</v>
+        <v>349</v>
       </c>
       <c r="C75" s="15" t="s">
         <v>156</v>
@@ -4243,10 +4237,10 @@
     </row>
     <row r="76" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A76" t="s">
-        <v>228</v>
+        <v>226</v>
       </c>
       <c r="B76" t="s">
-        <v>229</v>
+        <v>227</v>
       </c>
       <c r="C76" s="15" t="s">
         <v>158</v>
@@ -4266,10 +4260,10 @@
     </row>
     <row r="77" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A77" t="s">
-        <v>352</v>
+        <v>350</v>
       </c>
       <c r="B77" t="s">
-        <v>353</v>
+        <v>351</v>
       </c>
       <c r="C77" s="15" t="s">
         <v>160</v>
@@ -4289,10 +4283,10 @@
     </row>
     <row r="78" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A78" t="s">
-        <v>354</v>
+        <v>352</v>
       </c>
       <c r="B78" t="s">
-        <v>355</v>
+        <v>353</v>
       </c>
       <c r="C78" s="15" t="s">
         <v>162</v>
@@ -4312,10 +4306,10 @@
     </row>
     <row r="79" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A79" t="s">
-        <v>356</v>
+        <v>354</v>
       </c>
       <c r="B79" t="s">
-        <v>357</v>
+        <v>355</v>
       </c>
       <c r="C79" s="15" t="s">
         <v>164</v>
@@ -4335,10 +4329,10 @@
     </row>
     <row r="80" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A80" t="s">
-        <v>358</v>
+        <v>356</v>
       </c>
       <c r="B80" t="s">
-        <v>359</v>
+        <v>357</v>
       </c>
       <c r="C80" s="15" t="s">
         <v>166</v>
@@ -4358,10 +4352,10 @@
     </row>
     <row r="81" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A81" t="s">
-        <v>360</v>
+        <v>358</v>
       </c>
       <c r="B81" t="s">
-        <v>361</v>
+        <v>359</v>
       </c>
       <c r="C81" s="15" t="s">
         <v>168</v>
@@ -4381,10 +4375,10 @@
     </row>
     <row r="82" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A82" t="s">
-        <v>362</v>
+        <v>360</v>
       </c>
       <c r="B82" t="s">
-        <v>363</v>
+        <v>361</v>
       </c>
       <c r="C82" s="15" t="s">
         <v>170</v>
@@ -4404,10 +4398,10 @@
     </row>
     <row r="83" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A83" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
       <c r="B83" t="s">
-        <v>214</v>
+        <v>212</v>
       </c>
       <c r="C83" s="15" t="s">
         <v>172</v>
@@ -4433,9 +4427,11 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{998B2A50-6942-45EF-91DE-24539BE68CC0}">
-  <dimension ref="A1:F36"/>
+  <dimension ref="A1:F35"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A11" sqref="A11:XFD11"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
@@ -4568,10 +4564,10 @@
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A7" s="18" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
       <c r="B7" s="18" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
       <c r="C7" s="18">
         <v>1</v>
@@ -4583,15 +4579,15 @@
         <v>11</v>
       </c>
       <c r="F7" s="2" t="s">
-        <v>234</v>
+        <v>232</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A8" s="18" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
       <c r="B8" s="18" t="s">
-        <v>192</v>
+        <v>190</v>
       </c>
       <c r="C8" s="18">
         <v>1</v>
@@ -4603,15 +4599,15 @@
         <v>11</v>
       </c>
       <c r="F8" s="2" t="s">
-        <v>234</v>
+        <v>232</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A9" s="18" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
       <c r="B9" s="18" t="s">
-        <v>194</v>
+        <v>192</v>
       </c>
       <c r="C9" s="18">
         <v>6</v>
@@ -4623,15 +4619,15 @@
         <v>11</v>
       </c>
       <c r="F9" s="2" t="s">
-        <v>234</v>
+        <v>232</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A10" s="18" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
       <c r="B10" s="18" t="s">
-        <v>196</v>
+        <v>194</v>
       </c>
       <c r="C10" s="18">
         <v>6</v>
@@ -4643,27 +4639,27 @@
         <v>11</v>
       </c>
       <c r="F10" s="2" t="s">
-        <v>234</v>
+        <v>232</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A11" s="18" t="s">
-        <v>187</v>
+        <v>195</v>
       </c>
       <c r="B11" s="18" t="s">
-        <v>188</v>
+        <v>196</v>
       </c>
       <c r="C11" s="18">
-        <v>12</v>
+        <v>4</v>
       </c>
       <c r="D11" s="18">
-        <v>23665.26</v>
+        <v>9033.8799999999992</v>
       </c>
       <c r="E11" s="11" t="s">
         <v>11</v>
       </c>
       <c r="F11" s="2" t="s">
-        <v>234</v>
+        <v>232</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.3">
@@ -4677,53 +4673,53 @@
         <v>4</v>
       </c>
       <c r="D12" s="18">
-        <v>9033.8799999999992</v>
+        <v>4627.12</v>
       </c>
       <c r="E12" s="11" t="s">
         <v>11</v>
       </c>
       <c r="F12" s="2" t="s">
-        <v>234</v>
+        <v>232</v>
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A13" s="18" t="s">
-        <v>199</v>
+        <v>189</v>
       </c>
       <c r="B13" s="18" t="s">
-        <v>200</v>
+        <v>190</v>
       </c>
       <c r="C13" s="18">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="D13" s="18">
-        <v>4627.12</v>
+        <v>8014.83</v>
       </c>
       <c r="E13" s="11" t="s">
         <v>11</v>
       </c>
       <c r="F13" s="2" t="s">
-        <v>234</v>
+        <v>232</v>
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A14" s="18" t="s">
-        <v>191</v>
+        <v>199</v>
       </c>
       <c r="B14" s="18" t="s">
-        <v>192</v>
+        <v>200</v>
       </c>
       <c r="C14" s="18">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="D14" s="18">
-        <v>8014.83</v>
+        <v>1983.06</v>
       </c>
       <c r="E14" s="11" t="s">
         <v>11</v>
       </c>
       <c r="F14" s="2" t="s">
-        <v>234</v>
+        <v>232</v>
       </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.3">
@@ -4737,13 +4733,13 @@
         <v>2</v>
       </c>
       <c r="D15" s="18">
-        <v>1983.06</v>
+        <v>2864.4</v>
       </c>
       <c r="E15" s="11" t="s">
         <v>11</v>
       </c>
       <c r="F15" s="2" t="s">
-        <v>234</v>
+        <v>232</v>
       </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.3">
@@ -4754,16 +4750,16 @@
         <v>204</v>
       </c>
       <c r="C16" s="18">
-        <v>2</v>
+        <v>6</v>
       </c>
       <c r="D16" s="18">
-        <v>2864.4</v>
+        <v>15864.42</v>
       </c>
       <c r="E16" s="11" t="s">
         <v>11</v>
       </c>
       <c r="F16" s="2" t="s">
-        <v>234</v>
+        <v>232</v>
       </c>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.3">
@@ -4774,16 +4770,16 @@
         <v>206</v>
       </c>
       <c r="C17" s="18">
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="D17" s="18">
-        <v>15864.42</v>
+        <v>1983.06</v>
       </c>
       <c r="E17" s="11" t="s">
         <v>11</v>
       </c>
       <c r="F17" s="2" t="s">
-        <v>234</v>
+        <v>232</v>
       </c>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.3">
@@ -4794,16 +4790,16 @@
         <v>208</v>
       </c>
       <c r="C18" s="18">
-        <v>2</v>
+        <v>10</v>
       </c>
       <c r="D18" s="18">
-        <v>1983.06</v>
+        <v>22584.7</v>
       </c>
       <c r="E18" s="11" t="s">
         <v>11</v>
       </c>
       <c r="F18" s="2" t="s">
-        <v>234</v>
+        <v>232</v>
       </c>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.3">
@@ -4817,53 +4813,53 @@
         <v>10</v>
       </c>
       <c r="D19" s="18">
-        <v>22584.7</v>
+        <v>11567.8</v>
       </c>
       <c r="E19" s="11" t="s">
         <v>11</v>
       </c>
       <c r="F19" s="2" t="s">
-        <v>234</v>
+        <v>232</v>
       </c>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A20" s="18" t="s">
-        <v>211</v>
+        <v>174</v>
       </c>
       <c r="B20" s="18" t="s">
-        <v>212</v>
+        <v>175</v>
       </c>
       <c r="C20" s="18">
-        <v>10</v>
+        <v>1</v>
       </c>
       <c r="D20" s="18">
-        <v>11567.8</v>
+        <v>2258.4699999999998</v>
       </c>
       <c r="E20" s="11" t="s">
         <v>11</v>
       </c>
       <c r="F20" s="2" t="s">
-        <v>234</v>
+        <v>232</v>
       </c>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A21" s="18" t="s">
-        <v>174</v>
+        <v>211</v>
       </c>
       <c r="B21" s="18" t="s">
-        <v>175</v>
+        <v>212</v>
       </c>
       <c r="C21" s="18">
         <v>1</v>
       </c>
       <c r="D21" s="18">
-        <v>2258.4699999999998</v>
+        <v>2038.14</v>
       </c>
       <c r="E21" s="11" t="s">
         <v>11</v>
       </c>
       <c r="F21" s="2" t="s">
-        <v>234</v>
+        <v>232</v>
       </c>
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.3">
@@ -4871,39 +4867,39 @@
         <v>213</v>
       </c>
       <c r="B22" s="18" t="s">
-        <v>214</v>
+        <v>185</v>
       </c>
       <c r="C22" s="18">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="D22" s="18">
-        <v>2038.14</v>
+        <v>5783.9</v>
       </c>
       <c r="E22" s="11" t="s">
         <v>11</v>
       </c>
       <c r="F22" s="2" t="s">
-        <v>234</v>
+        <v>232</v>
       </c>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A23" s="18" t="s">
+        <v>214</v>
+      </c>
+      <c r="B23" s="18" t="s">
         <v>215</v>
       </c>
-      <c r="B23" s="18" t="s">
-        <v>185</v>
-      </c>
       <c r="C23" s="18">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="D23" s="18">
-        <v>5783.9</v>
+        <v>12063.54</v>
       </c>
       <c r="E23" s="11" t="s">
         <v>11</v>
       </c>
       <c r="F23" s="2" t="s">
-        <v>234</v>
+        <v>232</v>
       </c>
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.3">
@@ -4914,24 +4910,24 @@
         <v>217</v>
       </c>
       <c r="C24" s="18">
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="D24" s="18">
-        <v>12063.54</v>
+        <v>2313.56</v>
       </c>
       <c r="E24" s="11" t="s">
         <v>11</v>
       </c>
       <c r="F24" s="2" t="s">
-        <v>234</v>
+        <v>232</v>
       </c>
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A25" s="18" t="s">
-        <v>218</v>
+        <v>182</v>
       </c>
       <c r="B25" s="18" t="s">
-        <v>219</v>
+        <v>183</v>
       </c>
       <c r="C25" s="18">
         <v>2</v>
@@ -4943,27 +4939,27 @@
         <v>11</v>
       </c>
       <c r="F25" s="2" t="s">
-        <v>234</v>
+        <v>232</v>
       </c>
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A26" s="18" t="s">
-        <v>182</v>
+        <v>218</v>
       </c>
       <c r="B26" s="18" t="s">
-        <v>183</v>
+        <v>219</v>
       </c>
       <c r="C26" s="18">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="D26" s="18">
-        <v>2313.56</v>
+        <v>3305.07</v>
       </c>
       <c r="E26" s="11" t="s">
         <v>11</v>
       </c>
       <c r="F26" s="2" t="s">
-        <v>234</v>
+        <v>232</v>
       </c>
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.3">
@@ -4977,13 +4973,13 @@
         <v>3</v>
       </c>
       <c r="D27" s="18">
-        <v>3305.07</v>
+        <v>4627.1099999999997</v>
       </c>
       <c r="E27" s="11" t="s">
         <v>11</v>
       </c>
       <c r="F27" s="2" t="s">
-        <v>234</v>
+        <v>232</v>
       </c>
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.3">
@@ -4997,13 +4993,13 @@
         <v>3</v>
       </c>
       <c r="D28" s="18">
-        <v>4627.1099999999997</v>
+        <v>10906.77</v>
       </c>
       <c r="E28" s="11" t="s">
         <v>11</v>
       </c>
       <c r="F28" s="2" t="s">
-        <v>234</v>
+        <v>232</v>
       </c>
     </row>
     <row r="29" spans="1:6" x14ac:dyDescent="0.3">
@@ -5014,16 +5010,16 @@
         <v>225</v>
       </c>
       <c r="C29" s="18">
-        <v>3</v>
+        <v>7</v>
       </c>
       <c r="D29" s="18">
-        <v>10906.77</v>
+        <v>5398.33</v>
       </c>
       <c r="E29" s="11" t="s">
         <v>11</v>
       </c>
       <c r="F29" s="2" t="s">
-        <v>234</v>
+        <v>232</v>
       </c>
     </row>
     <row r="30" spans="1:6" x14ac:dyDescent="0.3">
@@ -5037,13 +5033,13 @@
         <v>7</v>
       </c>
       <c r="D30" s="18">
-        <v>5398.33</v>
+        <v>8097.46</v>
       </c>
       <c r="E30" s="11" t="s">
         <v>11</v>
       </c>
       <c r="F30" s="2" t="s">
-        <v>234</v>
+        <v>232</v>
       </c>
     </row>
     <row r="31" spans="1:6" x14ac:dyDescent="0.3">
@@ -5054,16 +5050,16 @@
         <v>229</v>
       </c>
       <c r="C31" s="18">
-        <v>7</v>
+        <v>2</v>
       </c>
       <c r="D31" s="18">
-        <v>8097.46</v>
+        <v>3854.84</v>
       </c>
       <c r="E31" s="11" t="s">
         <v>11</v>
       </c>
       <c r="F31" s="2" t="s">
-        <v>234</v>
+        <v>232</v>
       </c>
     </row>
     <row r="32" spans="1:6" x14ac:dyDescent="0.3">
@@ -5074,37 +5070,25 @@
         <v>231</v>
       </c>
       <c r="C32" s="18">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="D32" s="18">
-        <v>3854.84</v>
+        <v>2338.4</v>
       </c>
       <c r="E32" s="11" t="s">
         <v>11</v>
       </c>
       <c r="F32" s="2" t="s">
-        <v>234</v>
+        <v>232</v>
       </c>
     </row>
     <row r="33" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A33" s="18" t="s">
-        <v>232</v>
-      </c>
-      <c r="B33" s="18" t="s">
-        <v>233</v>
-      </c>
-      <c r="C33" s="18">
-        <v>5</v>
-      </c>
-      <c r="D33" s="18">
-        <v>2338.4</v>
-      </c>
-      <c r="E33" s="11" t="s">
-        <v>11</v>
-      </c>
-      <c r="F33" s="2" t="s">
-        <v>234</v>
-      </c>
+      <c r="A33" s="2"/>
+      <c r="B33" s="2"/>
+      <c r="C33" s="2"/>
+      <c r="D33" s="2"/>
+      <c r="E33" s="2"/>
+      <c r="F33" s="2"/>
     </row>
     <row r="34" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A34" s="2"/>
@@ -5122,14 +5106,6 @@
       <c r="E35" s="2"/>
       <c r="F35" s="2"/>
     </row>
-    <row r="36" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A36" s="2"/>
-      <c r="B36" s="2"/>
-      <c r="C36" s="2"/>
-      <c r="D36" s="2"/>
-      <c r="E36" s="2"/>
-      <c r="F36" s="2"/>
-    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>